<commit_message>
Retraced the lower PCB
</commit_message>
<xml_diff>
--- a/ThumbsUpV2_rp2040_BOM.xlsx
+++ b/ThumbsUpV2_rp2040_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak\Documents\GitHub\ThumbsUpUnsplitV2Rp2040\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C9640B-9F8D-4017-85C1-918F5D36B445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FEC868-1797-4794-A881-4A926716EA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{72E59EA4-12F0-45CA-99F5-811768B66A55}"/>
+    <workbookView xWindow="1380" yWindow="-15" windowWidth="11295" windowHeight="18030" xr2:uid="{72E59EA4-12F0-45CA-99F5-811768B66A55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Comment</t>
   </si>
@@ -85,9 +77,6 @@
     <t>TL1016AAF220QG</t>
   </si>
   <si>
-    <t>RUN,BOOTSEL</t>
-  </si>
-  <si>
     <t>RP2040</t>
   </si>
   <si>
@@ -106,15 +95,6 @@
     <t>D_SOD-123</t>
   </si>
   <si>
-    <t>ABLS-12.000MHZ-B4-T</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>HC%2f49US-(AT49)_1</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -196,10 +176,28 @@
     <t>Fuse_1206_3216Metric</t>
   </si>
   <si>
-    <t>Molex-0548190589</t>
-  </si>
-  <si>
-    <t>USB1</t>
+    <t>USB_C_Receptacle_Palconn_UTC16-G</t>
+  </si>
+  <si>
+    <t>R9,R8</t>
+  </si>
+  <si>
+    <t>J32</t>
+  </si>
+  <si>
+    <t>RUN1,BOOTSEL1</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>5.1k</t>
+  </si>
+  <si>
+    <t>USB_C_Receptacle_USB2.0</t>
+  </si>
+  <si>
+    <t>DNF</t>
   </si>
 </sst>
 </file>
@@ -234,15 +232,21 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -265,11 +269,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,9 +292,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB3DDED-DC32-4F0D-9C5B-0C6B84FDC4EF}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -624,195 +638,190 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3"/>
+      <c r="A3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3"/>
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="3"/>
+      <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="3"/>
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3"/>
+      <c r="A14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>